<commit_message>
last commit before i make a ne folder for asstests
</commit_message>
<xml_diff>
--- a/test_case_records.xlsx
+++ b/test_case_records.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>DoulaHoop test cases</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,11 +68,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>testdoula</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>testdoula1@test.com</t>
+    <t>Tracie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>te@test.com</t>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -455,7 +463,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="A1:XFD1048576"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -525,14 +533,14 @@
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +550,6 @@
     <hyperlink ref="H4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="72" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="2" manualBreakCount="2">
     <brk id="9" max="1048575" man="1"/>
     <brk id="10" max="1048575" man="1"/>

</xml_diff>